<commit_message>
BG Training Success Criteria changed back from weight diff to expected reward and  analysis updated
</commit_message>
<xml_diff>
--- a/Data/Experiments/02_Grasping/02_Grasping.xlsx
+++ b/Data/Experiments/02_Grasping/02_Grasping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geige\Documents\MasterThesisCode\SpikingLearningModel\Data\Experiments\02_Grasping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AFC7E2-0602-4050-8829-7E0DAB8EE2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1625E678-2553-4BA8-A59B-BB9CBA383C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1747" yWindow="1747" windowWidth="15391" windowHeight="9533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -291,7 +291,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +307,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +333,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -344,9 +389,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -629,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1297,19 +1354,19 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A12">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <v>35</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="7">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="7" t="s">
         <v>48</v>
       </c>
       <c r="F12" t="s">
@@ -1333,7 +1390,7 @@
       <c r="L12" s="5">
         <v>-5</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="9">
         <v>100</v>
       </c>
       <c r="N12" s="5">
@@ -1356,19 +1413,19 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A13">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="7">
         <v>35</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="7">
         <v>46</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="7" t="s">
         <v>48</v>
       </c>
       <c r="F13" t="s">
@@ -1415,19 +1472,19 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A14">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="7">
         <v>35</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="7">
         <v>86</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="7" t="s">
         <v>48</v>
       </c>
       <c r="F14" t="s">
@@ -1474,19 +1531,19 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A15">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="7">
         <v>35</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <v>116</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="7" t="s">
         <v>48</v>
       </c>
       <c r="F15" t="s">
@@ -1519,10 +1576,10 @@
       <c r="O15" s="5">
         <v>1000</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q15" s="2" t="s">
+      <c r="P15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q15" s="15" t="s">
         <v>74</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -1569,7 +1626,7 @@
       <c r="L16" s="5">
         <v>-5</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="8">
         <v>25</v>
       </c>
       <c r="N16" s="5">
@@ -1592,19 +1649,19 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A17">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="7">
         <v>35</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="7">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F17" t="s">
@@ -1651,19 +1708,19 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A18">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="7">
         <v>35</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="7">
         <v>46</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F18" t="s">
@@ -1710,25 +1767,25 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A19">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="7">
         <v>35</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="16">
         <v>86</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1769,78 +1826,78 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A20">
+      <c r="A20" s="18">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="18">
         <v>35</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="18">
         <v>116</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="J20" s="5">
-        <v>30</v>
-      </c>
-      <c r="K20" s="5">
-        <v>8</v>
-      </c>
-      <c r="L20" s="5">
+      <c r="H20" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="J20" s="20">
+        <v>30</v>
+      </c>
+      <c r="K20" s="20">
+        <v>8</v>
+      </c>
+      <c r="L20" s="20">
         <v>-5</v>
       </c>
-      <c r="M20" s="5">
-        <v>25</v>
-      </c>
-      <c r="N20" s="5">
-        <v>200</v>
-      </c>
-      <c r="O20" s="5">
-        <v>1000</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="R20" s="2" t="s">
+      <c r="M20" s="20">
+        <v>25</v>
+      </c>
+      <c r="N20" s="20">
+        <v>200</v>
+      </c>
+      <c r="O20" s="20">
+        <v>1000</v>
+      </c>
+      <c r="P20" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="R20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S20" t="s">
+      <c r="S20" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A21">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="7">
         <v>35</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="7">
         <v>116</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F21" t="s">
@@ -1896,16 +1953,16 @@
       <c r="C22">
         <v>35</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="16">
         <v>86</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="16" t="s">
         <v>55</v>
       </c>
       <c r="H22" s="4" t="s">
@@ -1967,40 +2024,40 @@
       <c r="G23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J23" s="8">
-        <v>30</v>
-      </c>
-      <c r="K23" s="8">
-        <v>8</v>
-      </c>
-      <c r="L23" s="8">
+      <c r="H23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J23" s="11">
+        <v>30</v>
+      </c>
+      <c r="K23" s="11">
+        <v>8</v>
+      </c>
+      <c r="L23" s="11">
         <v>-5</v>
       </c>
-      <c r="M23" s="8">
-        <v>25</v>
-      </c>
-      <c r="N23" s="8">
-        <v>200</v>
-      </c>
-      <c r="O23" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P23" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q23" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R23" s="9" t="s">
+      <c r="M23" s="11">
+        <v>25</v>
+      </c>
+      <c r="N23" s="11">
+        <v>200</v>
+      </c>
+      <c r="O23" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q23" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R23" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S23" s="6"/>
+      <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
@@ -2024,40 +2081,40 @@
       <c r="G24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J24" s="8">
-        <v>30</v>
-      </c>
-      <c r="K24" s="8">
-        <v>8</v>
-      </c>
-      <c r="L24" s="8">
+      <c r="H24" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J24" s="11">
+        <v>30</v>
+      </c>
+      <c r="K24" s="11">
+        <v>8</v>
+      </c>
+      <c r="L24" s="11">
         <v>-5</v>
       </c>
-      <c r="M24" s="8">
-        <v>25</v>
-      </c>
-      <c r="N24" s="8">
-        <v>200</v>
-      </c>
-      <c r="O24" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P24" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q24" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R24" s="9" t="s">
+      <c r="M24" s="11">
+        <v>25</v>
+      </c>
+      <c r="N24" s="11">
+        <v>200</v>
+      </c>
+      <c r="O24" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q24" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R24" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S24" s="6"/>
+      <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
@@ -2081,40 +2138,40 @@
       <c r="G25" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I25" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J25" s="8">
-        <v>30</v>
-      </c>
-      <c r="K25" s="8">
-        <v>8</v>
-      </c>
-      <c r="L25" s="8">
+      <c r="H25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J25" s="11">
+        <v>30</v>
+      </c>
+      <c r="K25" s="11">
+        <v>8</v>
+      </c>
+      <c r="L25" s="11">
         <v>-5</v>
       </c>
-      <c r="M25" s="8">
-        <v>25</v>
-      </c>
-      <c r="N25" s="8">
-        <v>200</v>
-      </c>
-      <c r="O25" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P25" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q25" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R25" s="9" t="s">
+      <c r="M25" s="11">
+        <v>25</v>
+      </c>
+      <c r="N25" s="11">
+        <v>200</v>
+      </c>
+      <c r="O25" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P25" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q25" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R25" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S25" s="6"/>
+      <c r="S25" s="13"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
@@ -2138,40 +2195,40 @@
       <c r="G26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J26" s="8">
-        <v>30</v>
-      </c>
-      <c r="K26" s="8">
-        <v>8</v>
-      </c>
-      <c r="L26" s="8">
+      <c r="H26" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J26" s="11">
+        <v>30</v>
+      </c>
+      <c r="K26" s="11">
+        <v>8</v>
+      </c>
+      <c r="L26" s="11">
         <v>-5</v>
       </c>
-      <c r="M26" s="8">
-        <v>25</v>
-      </c>
-      <c r="N26" s="8">
-        <v>200</v>
-      </c>
-      <c r="O26" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P26" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q26" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R26" s="9" t="s">
+      <c r="M26" s="11">
+        <v>25</v>
+      </c>
+      <c r="N26" s="11">
+        <v>200</v>
+      </c>
+      <c r="O26" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R26" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S26" s="6"/>
+      <c r="S26" s="13"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" s="6">
@@ -2195,40 +2252,40 @@
       <c r="G27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I27" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J27" s="8">
-        <v>30</v>
-      </c>
-      <c r="K27" s="8">
-        <v>8</v>
-      </c>
-      <c r="L27" s="8">
+      <c r="H27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J27" s="11">
+        <v>30</v>
+      </c>
+      <c r="K27" s="11">
+        <v>8</v>
+      </c>
+      <c r="L27" s="11">
         <v>-5</v>
       </c>
-      <c r="M27" s="8">
-        <v>25</v>
-      </c>
-      <c r="N27" s="8">
-        <v>200</v>
-      </c>
-      <c r="O27" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P27" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q27" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R27" s="9" t="s">
+      <c r="M27" s="11">
+        <v>25</v>
+      </c>
+      <c r="N27" s="11">
+        <v>200</v>
+      </c>
+      <c r="O27" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R27" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S27" s="6"/>
+      <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
@@ -2252,40 +2309,40 @@
       <c r="G28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J28" s="8">
-        <v>30</v>
-      </c>
-      <c r="K28" s="8">
-        <v>8</v>
-      </c>
-      <c r="L28" s="8">
+      <c r="H28" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J28" s="11">
+        <v>30</v>
+      </c>
+      <c r="K28" s="11">
+        <v>8</v>
+      </c>
+      <c r="L28" s="11">
         <v>-5</v>
       </c>
-      <c r="M28" s="8">
-        <v>25</v>
-      </c>
-      <c r="N28" s="8">
-        <v>200</v>
-      </c>
-      <c r="O28" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P28" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q28" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R28" s="9" t="s">
+      <c r="M28" s="11">
+        <v>25</v>
+      </c>
+      <c r="N28" s="11">
+        <v>200</v>
+      </c>
+      <c r="O28" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P28" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q28" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R28" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S28" s="6"/>
+      <c r="S28" s="13"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" s="6">
@@ -2309,40 +2366,40 @@
       <c r="G29" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J29" s="8">
-        <v>30</v>
-      </c>
-      <c r="K29" s="8">
-        <v>8</v>
-      </c>
-      <c r="L29" s="8">
+      <c r="H29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J29" s="11">
+        <v>30</v>
+      </c>
+      <c r="K29" s="11">
+        <v>8</v>
+      </c>
+      <c r="L29" s="11">
         <v>-5</v>
       </c>
-      <c r="M29" s="8">
-        <v>25</v>
-      </c>
-      <c r="N29" s="8">
-        <v>200</v>
-      </c>
-      <c r="O29" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P29" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q29" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R29" s="9" t="s">
+      <c r="M29" s="11">
+        <v>25</v>
+      </c>
+      <c r="N29" s="11">
+        <v>200</v>
+      </c>
+      <c r="O29" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R29" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S29" s="6" t="s">
+      <c r="S29" s="13" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2368,40 +2425,40 @@
       <c r="G30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J30" s="8">
-        <v>30</v>
-      </c>
-      <c r="K30" s="8">
-        <v>8</v>
-      </c>
-      <c r="L30" s="8">
+      <c r="H30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J30" s="11">
+        <v>30</v>
+      </c>
+      <c r="K30" s="11">
+        <v>8</v>
+      </c>
+      <c r="L30" s="11">
         <v>-5</v>
       </c>
-      <c r="M30" s="8">
-        <v>25</v>
-      </c>
-      <c r="N30" s="8">
-        <v>200</v>
-      </c>
-      <c r="O30" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P30" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q30" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R30" s="9" t="s">
+      <c r="M30" s="11">
+        <v>25</v>
+      </c>
+      <c r="N30" s="11">
+        <v>200</v>
+      </c>
+      <c r="O30" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P30" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q30" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R30" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S30" s="6" t="s">
+      <c r="S30" s="13" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2427,40 +2484,40 @@
       <c r="G31" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I31" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="J31" s="8">
-        <v>30</v>
-      </c>
-      <c r="K31" s="8">
-        <v>8</v>
-      </c>
-      <c r="L31" s="8">
+      <c r="H31" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="J31" s="11">
+        <v>30</v>
+      </c>
+      <c r="K31" s="11">
+        <v>8</v>
+      </c>
+      <c r="L31" s="11">
         <v>-5</v>
       </c>
-      <c r="M31" s="8">
-        <v>25</v>
-      </c>
-      <c r="N31" s="8">
-        <v>200</v>
-      </c>
-      <c r="O31" s="8">
-        <v>1000</v>
-      </c>
-      <c r="P31" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q31" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R31" s="9" t="s">
+      <c r="M31" s="11">
+        <v>25</v>
+      </c>
+      <c r="N31" s="11">
+        <v>200</v>
+      </c>
+      <c r="O31" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P31" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q31" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S31" s="6" t="s">
+      <c r="S31" s="13" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2468,22 +2525,22 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="17">
         <v>35</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="16">
         <v>86</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="16" t="s">
         <v>18</v>
       </c>
       <c r="H32" s="4" t="s">
@@ -2527,19 +2584,19 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="17">
         <v>35</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="17">
         <v>46</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="17" t="s">
         <v>60</v>
       </c>
       <c r="G33" t="s">
@@ -2586,19 +2643,19 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="17">
         <v>35</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="17">
         <v>46</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="17" t="s">
         <v>60</v>
       </c>
       <c r="G34" t="s">
@@ -2645,19 +2702,19 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="17">
         <v>35</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="14">
         <v>86</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="17" t="s">
         <v>60</v>
       </c>
       <c r="G35" t="s">
@@ -2687,10 +2744,10 @@
       <c r="O35" s="5">
         <v>1000</v>
       </c>
-      <c r="P35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q35" s="2" t="s">
+      <c r="P35" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="R35" s="2" t="s">
@@ -2710,10 +2767,10 @@
       <c r="C36">
         <v>35</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="14">
         <v>86</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="14" t="s">
         <v>48</v>
       </c>
       <c r="F36" t="s">
@@ -2746,10 +2803,10 @@
       <c r="O36" s="5">
         <v>1000</v>
       </c>
-      <c r="P36" s="2" t="s">
+      <c r="P36" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Q36" s="2" t="s">
+      <c r="Q36" s="15" t="s">
         <v>74</v>
       </c>
       <c r="R36" s="2" t="s">
@@ -2769,10 +2826,10 @@
       <c r="C37">
         <v>35</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="14">
         <v>86</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="14" t="s">
         <v>48</v>
       </c>
       <c r="F37" t="s">
@@ -2805,10 +2862,10 @@
       <c r="O37" s="5">
         <v>1000</v>
       </c>
-      <c r="P37" s="2" t="s">
+      <c r="P37" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Q37" s="2" t="s">
+      <c r="Q37" s="15" t="s">
         <v>16</v>
       </c>
       <c r="R37" s="2" t="s">
@@ -2828,10 +2885,10 @@
       <c r="C38">
         <v>35</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="14">
         <v>116</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="14" t="s">
         <v>48</v>
       </c>
       <c r="F38" t="s">
@@ -2864,10 +2921,10 @@
       <c r="O38" s="5">
         <v>1000</v>
       </c>
-      <c r="P38" s="2" t="s">
+      <c r="P38" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Q38" s="2" t="s">
+      <c r="Q38" s="15" t="s">
         <v>16</v>
       </c>
       <c r="R38" s="2" t="s">

</xml_diff>